<commit_message>
Add missing default and type values to code generation.
</commit_message>
<xml_diff>
--- a/codegeneration/queries.xlsx
+++ b/codegeneration/queries.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2831" uniqueCount="1024">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="1028">
   <si>
     <t>GL_MODELVIEW_MATRIX</t>
   </si>
@@ -3110,6 +3110,18 @@
   </si>
   <si>
     <t>glTexGen</t>
+  </si>
+  <si>
+    <t>glLoadTransposeMatrix</t>
+  </si>
+  <si>
+    <t>Transpose Matrix States</t>
+  </si>
+  <si>
+    <t>glBindVertexArray</t>
+  </si>
+  <si>
+    <t>Vertex Binding States</t>
   </si>
 </sst>
 </file>
@@ -3399,448 +3411,7 @@
     <cellStyle name="Prozent" xfId="3" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="169">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="106">
     <dxf>
       <fill>
         <patternFill>
@@ -4706,30 +4277,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table10" displayName="Table10" ref="A1:L591" totalsRowShown="0" headerRowDxfId="168" dataDxfId="167">
-  <autoFilter ref="A1:L591"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table10" displayName="Table10" ref="A1:L593" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
+  <autoFilter ref="A1:L593"/>
   <sortState ref="A2:J558">
     <sortCondition ref="A276"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="enum" dataDxfId="166"/>
-    <tableColumn id="2" name="description" dataDxfId="165"/>
-    <tableColumn id="3" name="group" dataDxfId="164"/>
-    <tableColumn id="9" name="function" dataDxfId="163"/>
-    <tableColumn id="4" name="default" dataDxfId="162"/>
-    <tableColumn id="14" name="status" dataDxfId="161">
+    <tableColumn id="1" name="enum" dataDxfId="103"/>
+    <tableColumn id="2" name="description" dataDxfId="102"/>
+    <tableColumn id="3" name="group" dataDxfId="101"/>
+    <tableColumn id="9" name="function" dataDxfId="100"/>
+    <tableColumn id="4" name="default" dataDxfId="99"/>
+    <tableColumn id="14" name="status" dataDxfId="98">
       <calculatedColumnFormula>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="type" dataDxfId="160"/>
-    <tableColumn id="6" name="#" dataDxfId="159"/>
-    <tableColumn id="8" name="c++ code" dataDxfId="158">
+    <tableColumn id="5" name="type" dataDxfId="97"/>
+    <tableColumn id="6" name="#" dataDxfId="96"/>
+    <tableColumn id="8" name="c++ code" dataDxfId="95">
       <calculatedColumnFormula>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G2&amp;", "&amp;H2&amp;"&gt;("&amp;A2&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="is enum" dataDxfId="157"/>
-    <tableColumn id="17" name="checked" dataDxfId="156">
+    <tableColumn id="16" name="is enum" dataDxfId="94"/>
+    <tableColumn id="17" name="checked" dataDxfId="93">
       <calculatedColumnFormula>FALSE</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Column1" dataDxfId="155">
+    <tableColumn id="7" name="Column1" dataDxfId="92">
       <calculatedColumnFormula>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4738,7 +4309,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table16" displayName="Table16" ref="A1:B458" totalsRowShown="0" headerRowDxfId="154" dataDxfId="153" tableBorderDxfId="152">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table16" displayName="Table16" ref="A1:B458" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90" tableBorderDxfId="89">
   <autoFilter ref="A1:B458">
     <filterColumn colId="1">
       <filters>
@@ -4750,8 +4321,8 @@
     <sortCondition ref="A2"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="parsed and unfified list of glGet enums from" dataDxfId="151"/>
-    <tableColumn id="2" name="is grouped in sheet1" dataDxfId="150">
+    <tableColumn id="1" name="parsed and unfified list of glGet enums from" dataDxfId="88"/>
+    <tableColumn id="2" name="is grouped in sheet1" dataDxfId="87">
       <calculatedColumnFormula>NOT(ISERROR(VLOOKUP(Table16[parsed and unfified list of glGet enums from],Table10[enum],1,FALSE)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4760,7 +4331,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table18" displayName="Table18" ref="D1:D458" totalsRowShown="0" headerRowDxfId="149" headerRowBorderDxfId="148" tableBorderDxfId="147">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table18" displayName="Table18" ref="D1:D458" totalsRowShown="0" headerRowDxfId="86" headerRowBorderDxfId="85" tableBorderDxfId="84">
   <autoFilter ref="D1:D458"/>
   <tableColumns count="1">
     <tableColumn id="1" name="copy of ungrouped glGet enums"/>
@@ -5056,10 +4627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O593"/>
+  <dimension ref="A1:O595"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A520" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G537" sqref="G537"/>
+    <sheetView tabSelected="1" topLeftCell="A568" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B590" sqref="B590"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -25369,7 +24940,9 @@
       </c>
     </row>
     <row r="523" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A523" s="33"/>
+      <c r="A523" s="33" t="s">
+        <v>1025</v>
+      </c>
       <c r="B523" s="2"/>
       <c r="C523" s="2"/>
       <c r="D523" s="10"/>
@@ -25382,7 +24955,7 @@
       <c r="H523" s="15"/>
       <c r="I523" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G523&amp;", "&amp;H523&amp;"&gt;("&amp;A523&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>std::cout &lt;&lt; std::endl &lt;&lt; "" &lt;&lt; std::endl;</v>
+        <v>std::cout &lt;&lt; std::endl &lt;&lt; "Transpose Matrix States" &lt;&lt; std::endl;</v>
       </c>
       <c r="J523" s="32" t="b">
         <f>FALSE</f>
@@ -25398,24 +24971,28 @@
       </c>
     </row>
     <row r="524" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A524" s="34" t="s">
-        <v>679</v>
+      <c r="A524" s="33" t="s">
+        <v>732</v>
       </c>
       <c r="B524" s="2"/>
       <c r="C524" s="2"/>
-      <c r="D524" s="2"/>
+      <c r="D524" s="2" t="s">
+        <v>1024</v>
+      </c>
       <c r="E524" s="9"/>
       <c r="F524" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G524" s="1"/>
+      <c r="G524" s="1" t="s">
+        <v>926</v>
+      </c>
       <c r="H524" s="15">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I524" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G524&amp;", "&amp;H524&amp;"&gt;("&amp;A524&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_TIMESTAMP);</v>
+        <v>requestState&lt;GLdouble , 16&gt;(GL_TRANSPOSE_COLOR_MATRIX);</v>
       </c>
       <c r="J524" s="4" t="b">
         <f>TRUE</f>
@@ -25427,28 +25004,32 @@
       </c>
       <c r="L524" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="525" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A525" s="33" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B525" s="2"/>
       <c r="C525" s="2"/>
-      <c r="D525" s="2"/>
+      <c r="D525" s="2" t="s">
+        <v>1024</v>
+      </c>
       <c r="E525" s="9"/>
       <c r="F525" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G525" s="1"/>
+      <c r="G525" s="1" t="s">
+        <v>926</v>
+      </c>
       <c r="H525" s="15">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I525" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G525&amp;", "&amp;H525&amp;"&gt;("&amp;A525&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_TRANSPOSE_COLOR_MATRIX);</v>
+        <v>requestState&lt;GLdouble , 16&gt;(GL_TRANSPOSE_MODELVIEW_MATRIX);</v>
       </c>
       <c r="J525" s="4" t="b">
         <f>TRUE</f>
@@ -25460,28 +25041,32 @@
       </c>
       <c r="L525" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="526" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A526" s="33" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B526" s="2"/>
       <c r="C526" s="2"/>
-      <c r="D526" s="2"/>
+      <c r="D526" s="2" t="s">
+        <v>1024</v>
+      </c>
       <c r="E526" s="9"/>
       <c r="F526" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G526" s="1"/>
+      <c r="G526" s="1" t="s">
+        <v>926</v>
+      </c>
       <c r="H526" s="15">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I526" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G526&amp;", "&amp;H526&amp;"&gt;("&amp;A526&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_TRANSPOSE_MODELVIEW_MATRIX);</v>
+        <v>requestState&lt;GLdouble , 16&gt;(GL_TRANSPOSE_PROJECTION_MATRIX);</v>
       </c>
       <c r="J526" s="4" t="b">
         <f>TRUE</f>
@@ -25493,28 +25078,32 @@
       </c>
       <c r="L526" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="527" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A527" s="33" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B527" s="2"/>
       <c r="C527" s="2"/>
-      <c r="D527" s="2"/>
+      <c r="D527" s="2" t="s">
+        <v>1024</v>
+      </c>
       <c r="E527" s="9"/>
       <c r="F527" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G527" s="1"/>
+      <c r="G527" s="1" t="s">
+        <v>926</v>
+      </c>
       <c r="H527" s="15">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I527" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G527&amp;", "&amp;H527&amp;"&gt;("&amp;A527&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_TRANSPOSE_PROJECTION_MATRIX);</v>
+        <v>requestState&lt;GLdouble , 16&gt;(GL_TRANSPOSE_TEXTURE_MATRIX);</v>
       </c>
       <c r="J527" s="4" t="b">
         <f>TRUE</f>
@@ -25526,40 +25115,38 @@
       </c>
       <c r="L527" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="528" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A528" s="33" t="s">
-        <v>735</v>
+        <v>1027</v>
       </c>
       <c r="B528" s="2"/>
       <c r="C528" s="2"/>
-      <c r="D528" s="2"/>
-      <c r="E528" s="9"/>
-      <c r="F528" s="4" t="b">
-        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
-        <v>1</v>
-      </c>
-      <c r="G528" s="1"/>
-      <c r="H528" s="15">
-        <v>1</v>
-      </c>
-      <c r="I528" s="1" t="str">
+      <c r="D528" s="10"/>
+      <c r="E528" s="39"/>
+      <c r="F528" s="40" t="b">
+        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
+        <v>0</v>
+      </c>
+      <c r="G528" s="41"/>
+      <c r="H528" s="42"/>
+      <c r="I528" s="41" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G528&amp;", "&amp;H528&amp;"&gt;("&amp;A528&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_TRANSPOSE_TEXTURE_MATRIX);</v>
-      </c>
-      <c r="J528" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="K528" s="8" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="L528" s="10">
-        <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>27</v>
+        <v>std::cout &lt;&lt; std::endl &lt;&lt; "Vertex Binding States" &lt;&lt; std::endl;</v>
+      </c>
+      <c r="J528" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K528" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="L528" s="26" t="str">
+        <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
+        <v/>
       </c>
     </row>
     <row r="529" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
@@ -25568,19 +25155,25 @@
       </c>
       <c r="B529" s="2"/>
       <c r="C529" s="2"/>
-      <c r="D529" s="2"/>
-      <c r="E529" s="9"/>
+      <c r="D529" s="2" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E529" s="9">
+        <v>0</v>
+      </c>
       <c r="F529" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G529" s="1"/>
+      <c r="G529" s="1" t="s">
+        <v>831</v>
+      </c>
       <c r="H529" s="15">
         <v>1</v>
       </c>
       <c r="I529" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G529&amp;", "&amp;H529&amp;"&gt;("&amp;A529&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_VERTEX_ARRAY_BINDING);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_VERTEX_ARRAY_BINDING, { { 0 } });</v>
       </c>
       <c r="J529" s="4" t="b">
         <f>TRUE</f>
@@ -25601,19 +25194,25 @@
       </c>
       <c r="B530" s="2"/>
       <c r="C530" s="2"/>
-      <c r="D530" s="2"/>
-      <c r="E530" s="9"/>
+      <c r="D530" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="E530" s="9">
+        <v>0</v>
+      </c>
       <c r="F530" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G530" s="1"/>
+      <c r="G530" s="1" t="s">
+        <v>831</v>
+      </c>
       <c r="H530" s="15">
         <v>1</v>
       </c>
       <c r="I530" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G530&amp;", "&amp;H530&amp;"&gt;("&amp;A530&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_VERTEX_ARRAY_BUFFER_BINDING);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_VERTEX_ARRAY_BUFFER_BINDING, { { 0 } });</v>
       </c>
       <c r="J530" s="4" t="b">
         <f>TRUE</f>
@@ -25640,13 +25239,15 @@
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G531" s="1"/>
+      <c r="G531" s="1" t="s">
+        <v>831</v>
+      </c>
       <c r="H531" s="15">
         <v>1</v>
       </c>
       <c r="I531" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G531&amp;", "&amp;H531&amp;"&gt;("&amp;A531&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_VERTEX_BINDING_DIVISOR);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_VERTEX_BINDING_DIVISOR);</v>
       </c>
       <c r="J531" s="4" t="b">
         <f>TRUE</f>
@@ -25673,13 +25274,15 @@
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G532" s="1"/>
+      <c r="G532" s="1" t="s">
+        <v>831</v>
+      </c>
       <c r="H532" s="15">
         <v>1</v>
       </c>
       <c r="I532" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G532&amp;", "&amp;H532&amp;"&gt;("&amp;A532&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_VERTEX_BINDING_OFFSET);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_VERTEX_BINDING_OFFSET);</v>
       </c>
       <c r="J532" s="4" t="b">
         <f>TRUE</f>
@@ -25706,13 +25309,15 @@
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G533" s="1"/>
+      <c r="G533" s="1" t="s">
+        <v>831</v>
+      </c>
       <c r="H533" s="15">
         <v>1</v>
       </c>
       <c r="I533" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G533&amp;", "&amp;H533&amp;"&gt;("&amp;A533&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_VERTEX_BINDING_STRIDE);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_VERTEX_BINDING_STRIDE);</v>
       </c>
       <c r="J533" s="4" t="b">
         <f>TRUE</f>
@@ -25727,71 +25332,73 @@
         <v>24</v>
       </c>
     </row>
-    <row r="534" spans="1:12" ht="19.149999999999999" customHeight="1">
-      <c r="A534" s="33" t="s">
-        <v>571</v>
-      </c>
-      <c r="B534" s="10"/>
-      <c r="C534" s="10"/>
+    <row r="534" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
+      <c r="A534" s="34"/>
+      <c r="B534" s="2"/>
+      <c r="C534" s="2"/>
       <c r="D534" s="10"/>
-      <c r="E534" s="28"/>
-      <c r="F534" s="29" t="b">
-        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
-        <v>1</v>
-      </c>
-      <c r="G534" s="30"/>
-      <c r="H534" s="31"/>
-      <c r="I534" s="30" t="str">
+      <c r="E534" s="39"/>
+      <c r="F534" s="40" t="b">
+        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
+        <v>0</v>
+      </c>
+      <c r="G534" s="41"/>
+      <c r="H534" s="42"/>
+      <c r="I534" s="41" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G534&amp;", "&amp;H534&amp;"&gt;("&amp;A534&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, &gt;(GL_VERTEX_PROGRAM_POINT_SIZE);</v>
-      </c>
-      <c r="J534" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <v>std::cout &lt;&lt; std::endl &lt;&lt; "" &lt;&lt; std::endl;</v>
+      </c>
+      <c r="J534" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="K534" s="32" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="L534" s="10">
-        <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="535" spans="1:12" ht="19.149999999999999" customHeight="1">
+      <c r="L534" s="26" t="str">
+        <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="535" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A535" s="33" t="s">
-        <v>572</v>
-      </c>
-      <c r="B535" s="10"/>
-      <c r="C535" s="10"/>
-      <c r="D535" s="10"/>
-      <c r="E535" s="28"/>
-      <c r="F535" s="29" t="b">
-        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
-        <v>1</v>
-      </c>
-      <c r="G535" s="30"/>
-      <c r="H535" s="31"/>
-      <c r="I535" s="30" t="str">
+        <v>410</v>
+      </c>
+      <c r="B535" s="2"/>
+      <c r="C535" s="2"/>
+      <c r="D535" s="2"/>
+      <c r="E535" s="9"/>
+      <c r="F535" s="4" t="b">
+        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
+        <v>1</v>
+      </c>
+      <c r="G535" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="H535" s="15">
+        <v>2</v>
+      </c>
+      <c r="I535" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G535&amp;", "&amp;H535&amp;"&gt;("&amp;A535&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, &gt;(GL_VERTEX_PROGRAM_TWO_SIDE);</v>
+        <v>requestState&lt;GLfloat  , 2&gt;(GL_ALIASED_POINT_SIZE_RANGE);</v>
       </c>
       <c r="J535" s="4" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="K535" s="32" t="b">
+      <c r="K535" s="8" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="L535" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="536" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A536" s="33" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
       <c r="B536" s="2"/>
       <c r="C536" s="2"/>
@@ -25801,13 +25408,15 @@
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G536" s="1"/>
+      <c r="G536" s="1" t="s">
+        <v>830</v>
+      </c>
       <c r="H536" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I536" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G536&amp;", "&amp;H536&amp;"&gt;("&amp;A536&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 2&gt;(GL_ALIASED_POINT_SIZE_RANGE);</v>
+        <v>requestState&lt;GLboolean, 1&gt;(GL_COLOR_TABLE);</v>
       </c>
       <c r="J536" s="4" t="b">
         <f>TRUE</f>
@@ -25819,12 +25428,12 @@
       </c>
       <c r="L536" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="537" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A537" s="33" t="s">
-        <v>428</v>
+        <v>592</v>
       </c>
       <c r="B537" s="2"/>
       <c r="C537" s="2"/>
@@ -25835,14 +25444,14 @@
         <v>1</v>
       </c>
       <c r="G537" s="1" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="H537" s="15">
         <v>1</v>
       </c>
       <c r="I537" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G537&amp;", "&amp;H537&amp;"&gt;("&amp;A537&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLboolean, 1&gt;(GL_COLOR_TABLE);</v>
+        <v>requestState&lt;GLenum   , 1&gt;(GL_CONTEXT_FLAGS);</v>
       </c>
       <c r="J537" s="4" t="b">
         <f>TRUE</f>
@@ -25854,30 +25463,34 @@
       </c>
       <c r="L537" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="538" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A538" s="33" t="s">
-        <v>592</v>
+        <v>700</v>
       </c>
       <c r="B538" s="2"/>
       <c r="C538" s="2"/>
-      <c r="D538" s="2"/>
-      <c r="E538" s="9"/>
+      <c r="D538" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="E538" s="9">
+        <v>0</v>
+      </c>
       <c r="F538" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G538" s="1" t="s">
-        <v>833</v>
+        <v>926</v>
       </c>
       <c r="H538" s="15">
         <v>1</v>
       </c>
       <c r="I538" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G538&amp;", "&amp;H538&amp;"&gt;("&amp;A538&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLenum   , 1&gt;(GL_CONTEXT_FLAGS);</v>
+        <v>requestState&lt;GLdouble , 1&gt;(GL_CURRENT_FOG_COORD, { { 0 } });</v>
       </c>
       <c r="J538" s="4" t="b">
         <f>TRUE</f>
@@ -25889,34 +25502,32 @@
       </c>
       <c r="L538" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="539" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A539" s="33" t="s">
-        <v>700</v>
+        <v>593</v>
       </c>
       <c r="B539" s="2"/>
       <c r="C539" s="2"/>
       <c r="D539" s="2" t="s">
-        <v>927</v>
-      </c>
-      <c r="E539" s="9">
-        <v>0</v>
-      </c>
+        <v>930</v>
+      </c>
+      <c r="E539" s="9"/>
       <c r="F539" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G539" s="1" t="s">
-        <v>926</v>
+        <v>831</v>
       </c>
       <c r="H539" s="15">
         <v>1</v>
       </c>
       <c r="I539" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G539&amp;", "&amp;H539&amp;"&gt;("&amp;A539&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLdouble , 1&gt;(GL_CURRENT_FOG_COORD, { { 0 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_CURRENT_PROGRAM);</v>
       </c>
       <c r="J539" s="4" t="b">
         <f>TRUE</f>
@@ -25928,18 +25539,16 @@
       </c>
       <c r="L539" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="540" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A540" s="33" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B540" s="2"/>
       <c r="C540" s="2"/>
-      <c r="D540" s="2" t="s">
-        <v>930</v>
-      </c>
+      <c r="D540" s="2"/>
       <c r="E540" s="9"/>
       <c r="F540" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
@@ -25953,7 +25562,7 @@
       </c>
       <c r="I540" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G540&amp;", "&amp;H540&amp;"&gt;("&amp;A540&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_CURRENT_PROGRAM);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_DEBUG_GROUP_STACK_DEPTH);</v>
       </c>
       <c r="J540" s="4" t="b">
         <f>TRUE</f>
@@ -25965,30 +25574,36 @@
       </c>
       <c r="L540" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="541" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A541" s="33" t="s">
-        <v>591</v>
-      </c>
-      <c r="B541" s="2"/>
+      <c r="A541" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B541" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C541" s="2"/>
-      <c r="D541" s="2"/>
-      <c r="E541" s="9"/>
+      <c r="D541" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="E541" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="F541" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G541" s="1" t="s">
-        <v>831</v>
+        <v>834</v>
       </c>
       <c r="H541" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I541" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G541&amp;", "&amp;H541&amp;"&gt;("&amp;A541&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_DEBUG_GROUP_STACK_DEPTH);</v>
+        <v>requestState&lt;GLfloat  , 2&gt;(GL_DEPTH_RANGE, { { 0, 1 } });</v>
       </c>
       <c r="J541" s="4" t="b">
         <f>TRUE</f>
@@ -26000,36 +25615,32 @@
       </c>
       <c r="L541" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="542" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A542" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B542" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A542" s="33" t="s">
+        <v>443</v>
+      </c>
+      <c r="B542" s="2"/>
       <c r="C542" s="2"/>
-      <c r="D542" s="2" t="s">
-        <v>885</v>
-      </c>
+      <c r="D542" s="2"/>
       <c r="E542" s="9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F542" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G542" s="1" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="H542" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I542" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G542&amp;", "&amp;H542&amp;"&gt;("&amp;A542&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLfloat  , 2&gt;(GL_DEPTH_RANGE, { { 0, 1 } });</v>
+        <v>requestState&lt;GLboolean, 1&gt;(GL_HISTOGRAM, { { GL_FALSE } });</v>
       </c>
       <c r="J542" s="4" t="b">
         <f>TRUE</f>
@@ -26041,32 +25652,34 @@
       </c>
       <c r="L542" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="543" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A543" s="33" t="s">
-        <v>443</v>
+        <v>467</v>
       </c>
       <c r="B543" s="2"/>
       <c r="C543" s="2"/>
-      <c r="D543" s="2"/>
-      <c r="E543" s="9" t="s">
-        <v>18</v>
+      <c r="D543" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="E543" s="9">
+        <v>64</v>
       </c>
       <c r="F543" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G543" s="1" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="H543" s="15">
         <v>1</v>
       </c>
       <c r="I543" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G543&amp;", "&amp;H543&amp;"&gt;("&amp;A543&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLboolean, 1&gt;(GL_HISTOGRAM, { { GL_FALSE } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_3D_TEXTURE_SIZE, { { 64 } });</v>
       </c>
       <c r="J543" s="4" t="b">
         <f>TRUE</f>
@@ -26078,28 +25691,34 @@
       </c>
       <c r="L543" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="544" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A544" s="33" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B544" s="2"/>
       <c r="C544" s="2"/>
-      <c r="D544" s="2"/>
-      <c r="E544" s="9"/>
+      <c r="D544" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="E544" s="9">
+        <v>256</v>
+      </c>
       <c r="F544" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G544" s="1"/>
+      <c r="G544" s="1" t="s">
+        <v>831</v>
+      </c>
       <c r="H544" s="15">
         <v>1</v>
       </c>
       <c r="I544" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G544&amp;", "&amp;H544&amp;"&gt;("&amp;A544&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_MAJOR_VERSION);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_ARRAY_TEXTURE_LAYERS, { { 256 } });</v>
       </c>
       <c r="J544" s="4" t="b">
         <f>TRUE</f>
@@ -26111,28 +25730,32 @@
       </c>
       <c r="L544" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="545" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A545" s="34" t="s">
-        <v>652</v>
+      <c r="A545" s="33" t="s">
+        <v>601</v>
       </c>
       <c r="B545" s="2"/>
       <c r="C545" s="2"/>
       <c r="D545" s="2"/>
-      <c r="E545" s="9"/>
+      <c r="E545" s="9">
+        <v>8</v>
+      </c>
       <c r="F545" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G545" s="1"/>
+      <c r="G545" s="1" t="s">
+        <v>834</v>
+      </c>
       <c r="H545" s="15">
         <v>1</v>
       </c>
       <c r="I545" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G545&amp;", "&amp;H545&amp;"&gt;("&amp;A545&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_MINOR_VERSION);</v>
+        <v>requestState&lt;GLfloat  , 1&gt;(GL_MAX_CLIP_DISTANCES, { { 8 } });</v>
       </c>
       <c r="J545" s="4" t="b">
         <f>TRUE</f>
@@ -26144,21 +25767,17 @@
       </c>
       <c r="L545" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="546" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A546" s="33" t="s">
-        <v>467</v>
+        <v>602</v>
       </c>
       <c r="B546" s="2"/>
       <c r="C546" s="2"/>
-      <c r="D546" s="2" t="s">
-        <v>965</v>
-      </c>
-      <c r="E546" s="9">
-        <v>64</v>
-      </c>
+      <c r="D546" s="2"/>
+      <c r="E546" s="9"/>
       <c r="F546" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -26171,7 +25790,7 @@
       </c>
       <c r="I546" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G546&amp;", "&amp;H546&amp;"&gt;("&amp;A546&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_3D_TEXTURE_SIZE, { { 64 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_COLOR_TEXTURE_SAMPLES);</v>
       </c>
       <c r="J546" s="4" t="b">
         <f>TRUE</f>
@@ -26183,21 +25802,17 @@
       </c>
       <c r="L546" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="547" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A547" s="33" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="B547" s="2"/>
       <c r="C547" s="2"/>
-      <c r="D547" s="2" t="s">
-        <v>966</v>
-      </c>
-      <c r="E547" s="9">
-        <v>256</v>
-      </c>
+      <c r="D547" s="2"/>
+      <c r="E547" s="9"/>
       <c r="F547" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -26210,7 +25825,7 @@
       </c>
       <c r="I547" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G547&amp;", "&amp;H547&amp;"&gt;("&amp;A547&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_ARRAY_TEXTURE_LAYERS, { { 256 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_COMBINED_ATOMIC_COUNTERS);</v>
       </c>
       <c r="J547" s="4" t="b">
         <f>TRUE</f>
@@ -26222,32 +25837,30 @@
       </c>
       <c r="L547" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="548" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A548" s="33" t="s">
-        <v>601</v>
+        <v>579</v>
       </c>
       <c r="B548" s="2"/>
       <c r="C548" s="2"/>
       <c r="D548" s="2"/>
-      <c r="E548" s="9">
-        <v>8</v>
-      </c>
+      <c r="E548" s="9"/>
       <c r="F548" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G548" s="1" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="H548" s="15">
         <v>1</v>
       </c>
       <c r="I548" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G548&amp;", "&amp;H548&amp;"&gt;("&amp;A548&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLfloat  , 1&gt;(GL_MAX_CLIP_DISTANCES, { { 8 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_COMBINED_SHADER_STORAGE_BLOCKS);</v>
       </c>
       <c r="J548" s="4" t="b">
         <f>TRUE</f>
@@ -26259,17 +25872,21 @@
       </c>
       <c r="L548" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="549" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A549" s="33" t="s">
-        <v>602</v>
+        <v>470</v>
       </c>
       <c r="B549" s="2"/>
       <c r="C549" s="2"/>
-      <c r="D549" s="2"/>
-      <c r="E549" s="9"/>
+      <c r="D549" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="E549" s="9">
+        <v>1024</v>
+      </c>
       <c r="F549" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -26282,7 +25899,7 @@
       </c>
       <c r="I549" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G549&amp;", "&amp;H549&amp;"&gt;("&amp;A549&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_COLOR_TEXTURE_SAMPLES);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_CUBE_MAP_TEXTURE_SIZE, { { 1024 } });</v>
       </c>
       <c r="J549" s="4" t="b">
         <f>TRUE</f>
@@ -26299,7 +25916,7 @@
     </row>
     <row r="550" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A550" s="33" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="B550" s="2"/>
       <c r="C550" s="2"/>
@@ -26317,7 +25934,7 @@
       </c>
       <c r="I550" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G550&amp;", "&amp;H550&amp;"&gt;("&amp;A550&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_COMBINED_ATOMIC_COUNTERS);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_DEBUG_GROUP_STACK_DEPTH);</v>
       </c>
       <c r="J550" s="4" t="b">
         <f>TRUE</f>
@@ -26329,12 +25946,12 @@
       </c>
       <c r="L550" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="551" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A551" s="33" t="s">
-        <v>579</v>
+        <v>608</v>
       </c>
       <c r="B551" s="2"/>
       <c r="C551" s="2"/>
@@ -26352,7 +25969,7 @@
       </c>
       <c r="I551" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G551&amp;", "&amp;H551&amp;"&gt;("&amp;A551&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_COMBINED_SHADER_STORAGE_BLOCKS);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_DEPTH_TEXTURE_SAMPLES);</v>
       </c>
       <c r="J551" s="4" t="b">
         <f>TRUE</f>
@@ -26364,21 +25981,17 @@
       </c>
       <c r="L551" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="552" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A552" s="33" t="s">
-        <v>470</v>
+      <c r="A552" s="34" t="s">
+        <v>472</v>
       </c>
       <c r="B552" s="2"/>
       <c r="C552" s="2"/>
-      <c r="D552" s="2" t="s">
-        <v>966</v>
-      </c>
-      <c r="E552" s="9">
-        <v>1024</v>
-      </c>
+      <c r="D552" s="2"/>
+      <c r="E552" s="9"/>
       <c r="F552" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -26391,7 +26004,7 @@
       </c>
       <c r="I552" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G552&amp;", "&amp;H552&amp;"&gt;("&amp;A552&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_CUBE_MAP_TEXTURE_SIZE, { { 1024 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_ELEMENT_INDEX);</v>
       </c>
       <c r="J552" s="4" t="b">
         <f>TRUE</f>
@@ -26403,12 +26016,12 @@
       </c>
       <c r="L552" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="553" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A553" s="33" t="s">
-        <v>590</v>
+        <v>626</v>
       </c>
       <c r="B553" s="2"/>
       <c r="C553" s="2"/>
@@ -26426,7 +26039,7 @@
       </c>
       <c r="I553" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G553&amp;", "&amp;H553&amp;"&gt;("&amp;A553&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_DEBUG_GROUP_STACK_DEPTH);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_INTEGER_SAMPLES);</v>
       </c>
       <c r="J553" s="4" t="b">
         <f>TRUE</f>
@@ -26438,16 +26051,18 @@
       </c>
       <c r="L553" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="554" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A554" s="33" t="s">
-        <v>608</v>
+        <v>628</v>
       </c>
       <c r="B554" s="2"/>
       <c r="C554" s="2"/>
-      <c r="D554" s="2"/>
+      <c r="D554" s="2" t="s">
+        <v>982</v>
+      </c>
       <c r="E554" s="9"/>
       <c r="F554" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
@@ -26461,7 +26076,7 @@
       </c>
       <c r="I554" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G554&amp;", "&amp;H554&amp;"&gt;("&amp;A554&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_DEPTH_TEXTURE_SAMPLES);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_LABEL_LENGTH);</v>
       </c>
       <c r="J554" s="4" t="b">
         <f>TRUE</f>
@@ -26473,17 +26088,21 @@
       </c>
       <c r="L554" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="555" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A555" s="34" t="s">
-        <v>472</v>
+      <c r="A555" s="33" t="s">
+        <v>631</v>
       </c>
       <c r="B555" s="2"/>
       <c r="C555" s="2"/>
-      <c r="D555" s="2"/>
-      <c r="E555" s="9"/>
+      <c r="D555" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="E555" s="9">
+        <v>1024</v>
+      </c>
       <c r="F555" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -26496,7 +26115,7 @@
       </c>
       <c r="I555" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G555&amp;", "&amp;H555&amp;"&gt;("&amp;A555&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_ELEMENT_INDEX);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_RECTANGLE_TEXTURE_SIZE, { { 1024 } });</v>
       </c>
       <c r="J555" s="4" t="b">
         <f>TRUE</f>
@@ -26508,16 +26127,18 @@
       </c>
       <c r="L555" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="556" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A556" s="33" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="B556" s="2"/>
       <c r="C556" s="2"/>
-      <c r="D556" s="2"/>
+      <c r="D556" s="2" t="s">
+        <v>984</v>
+      </c>
       <c r="E556" s="9"/>
       <c r="F556" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
@@ -26531,7 +26152,7 @@
       </c>
       <c r="I556" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G556&amp;", "&amp;H556&amp;"&gt;("&amp;A556&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_INTEGER_SAMPLES);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_RENDERBUFFER_SIZE);</v>
       </c>
       <c r="J556" s="4" t="b">
         <f>TRUE</f>
@@ -26543,18 +26164,16 @@
       </c>
       <c r="L556" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="557" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A557" s="33" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
       <c r="B557" s="2"/>
       <c r="C557" s="2"/>
-      <c r="D557" s="2" t="s">
-        <v>982</v>
-      </c>
+      <c r="D557" s="2"/>
       <c r="E557" s="9"/>
       <c r="F557" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
@@ -26568,7 +26187,7 @@
       </c>
       <c r="I557" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G557&amp;", "&amp;H557&amp;"&gt;("&amp;A557&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_LABEL_LENGTH);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_SAMPLE_MASK_WORDS);</v>
       </c>
       <c r="J557" s="4" t="b">
         <f>TRUE</f>
@@ -26580,21 +26199,17 @@
       </c>
       <c r="L557" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="558" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A558" s="33" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="B558" s="2"/>
       <c r="C558" s="2"/>
-      <c r="D558" s="2" t="s">
-        <v>966</v>
-      </c>
-      <c r="E558" s="9">
-        <v>1024</v>
-      </c>
+      <c r="D558" s="2"/>
+      <c r="E558" s="9"/>
       <c r="F558" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -26607,7 +26222,7 @@
       </c>
       <c r="I558" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G558&amp;", "&amp;H558&amp;"&gt;("&amp;A558&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_RECTANGLE_TEXTURE_SIZE, { { 1024 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_SERVER_WAIT_TIMEOUT);</v>
       </c>
       <c r="J558" s="4" t="b">
         <f>TRUE</f>
@@ -26619,19 +26234,19 @@
       </c>
       <c r="L558" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="559" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A559" s="33" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="B559" s="2"/>
       <c r="C559" s="2"/>
-      <c r="D559" s="2" t="s">
-        <v>984</v>
-      </c>
-      <c r="E559" s="9"/>
+      <c r="D559" s="2"/>
+      <c r="E559" s="9">
+        <v>8</v>
+      </c>
       <c r="F559" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -26644,7 +26259,7 @@
       </c>
       <c r="I559" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G559&amp;", "&amp;H559&amp;"&gt;("&amp;A559&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_RENDERBUFFER_SIZE);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_SHADER_STORAGE_BUFFER_BINDINGS, { { 8 } });</v>
       </c>
       <c r="J559" s="4" t="b">
         <f>TRUE</f>
@@ -26656,17 +26271,19 @@
       </c>
       <c r="L559" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="560" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A560" s="33" t="s">
-        <v>633</v>
+        <v>642</v>
       </c>
       <c r="B560" s="2"/>
       <c r="C560" s="2"/>
       <c r="D560" s="2"/>
-      <c r="E560" s="9"/>
+      <c r="E560" s="9">
+        <v>16384</v>
+      </c>
       <c r="F560" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -26679,7 +26296,7 @@
       </c>
       <c r="I560" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G560&amp;", "&amp;H560&amp;"&gt;("&amp;A560&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_SAMPLE_MASK_WORDS);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_UNIFORM_BLOCK_SIZE, { { 16384 } });</v>
       </c>
       <c r="J560" s="4" t="b">
         <f>TRUE</f>
@@ -26691,17 +26308,19 @@
       </c>
       <c r="L560" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="561" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A561" s="33" t="s">
-        <v>634</v>
+        <v>641</v>
       </c>
       <c r="B561" s="2"/>
       <c r="C561" s="2"/>
       <c r="D561" s="2"/>
-      <c r="E561" s="9"/>
+      <c r="E561" s="9">
+        <v>36</v>
+      </c>
       <c r="F561" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -26714,7 +26333,7 @@
       </c>
       <c r="I561" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G561&amp;", "&amp;H561&amp;"&gt;("&amp;A561&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_SERVER_WAIT_TIMEOUT);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_UNIFORM_BUFFER_BINDINGS, { { 36 } });</v>
       </c>
       <c r="J561" s="4" t="b">
         <f>TRUE</f>
@@ -26726,18 +26345,18 @@
       </c>
       <c r="L561" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="562" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A562" s="33" t="s">
-        <v>635</v>
+        <v>643</v>
       </c>
       <c r="B562" s="2"/>
       <c r="C562" s="2"/>
       <c r="D562" s="2"/>
       <c r="E562" s="9">
-        <v>8</v>
+        <v>1024</v>
       </c>
       <c r="F562" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
@@ -26751,7 +26370,7 @@
       </c>
       <c r="I562" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G562&amp;", "&amp;H562&amp;"&gt;("&amp;A562&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_SHADER_STORAGE_BUFFER_BINDINGS, { { 8 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_UNIFORM_LOCATIONS, { { 1024 } });</v>
       </c>
       <c r="J562" s="4" t="b">
         <f>TRUE</f>
@@ -26763,18 +26382,18 @@
       </c>
       <c r="L562" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="563" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A563" s="33" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="B563" s="2"/>
       <c r="C563" s="2"/>
       <c r="D563" s="2"/>
       <c r="E563" s="9">
-        <v>16384</v>
+        <v>60</v>
       </c>
       <c r="F563" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
@@ -26788,7 +26407,7 @@
       </c>
       <c r="I563" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G563&amp;", "&amp;H563&amp;"&gt;("&amp;A563&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_UNIFORM_BLOCK_SIZE, { { 16384 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_VARYING_COMPONENTS, { { 60 } });</v>
       </c>
       <c r="J563" s="4" t="b">
         <f>TRUE</f>
@@ -26805,13 +26424,13 @@
     </row>
     <row r="564" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A564" s="33" t="s">
-        <v>641</v>
+        <v>480</v>
       </c>
       <c r="B564" s="2"/>
       <c r="C564" s="2"/>
       <c r="D564" s="2"/>
       <c r="E564" s="9">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F564" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
@@ -26825,7 +26444,7 @@
       </c>
       <c r="I564" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G564&amp;", "&amp;H564&amp;"&gt;("&amp;A564&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_UNIFORM_BUFFER_BINDINGS, { { 36 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_VARYING_FLOATS, { { 32 } });</v>
       </c>
       <c r="J564" s="4" t="b">
         <f>TRUE</f>
@@ -26837,18 +26456,18 @@
       </c>
       <c r="L564" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="565" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A565" s="33" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="B565" s="2"/>
       <c r="C565" s="2"/>
       <c r="D565" s="2"/>
       <c r="E565" s="9">
-        <v>1024</v>
+        <v>15</v>
       </c>
       <c r="F565" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
@@ -26862,7 +26481,7 @@
       </c>
       <c r="I565" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G565&amp;", "&amp;H565&amp;"&gt;("&amp;A565&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_UNIFORM_LOCATIONS, { { 1024 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_VARYING_VECTORS, { { 15 } });</v>
       </c>
       <c r="J565" s="4" t="b">
         <f>TRUE</f>
@@ -26874,18 +26493,20 @@
       </c>
       <c r="L565" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="566" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A566" s="33" t="s">
-        <v>644</v>
+        <v>627</v>
       </c>
       <c r="B566" s="2"/>
       <c r="C566" s="2"/>
-      <c r="D566" s="2"/>
+      <c r="D566" s="2" t="s">
+        <v>992</v>
+      </c>
       <c r="E566" s="9">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F566" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
@@ -26899,7 +26520,7 @@
       </c>
       <c r="I566" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G566&amp;", "&amp;H566&amp;"&gt;("&amp;A566&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_VARYING_COMPONENTS, { { 60 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_MIN_MAP_BUFFER_ALIGNMENT, { { 64 } });</v>
       </c>
       <c r="J566" s="4" t="b">
         <f>TRUE</f>
@@ -26911,32 +26532,34 @@
       </c>
       <c r="L566" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="567" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A567" s="33" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="B567" s="2"/>
       <c r="C567" s="2"/>
-      <c r="D567" s="2"/>
-      <c r="E567" s="9">
-        <v>32</v>
+      <c r="D567" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="E567" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="F567" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G567" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="H567" s="15">
         <v>1</v>
       </c>
       <c r="I567" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G567&amp;", "&amp;H567&amp;"&gt;("&amp;A567&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_VARYING_FLOATS, { { 32 } });</v>
+        <v>requestState&lt;GLboolean, 1&gt;(GL_MINMAX, { { GL_FALSE } });</v>
       </c>
       <c r="J567" s="4" t="b">
         <f>TRUE</f>
@@ -26948,32 +26571,36 @@
       </c>
       <c r="L567" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="568" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A568" s="33" t="s">
-        <v>645</v>
-      </c>
-      <c r="B568" s="2"/>
-      <c r="C568" s="2"/>
+      <c r="A568" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B568" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C568" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D568" s="2"/>
-      <c r="E568" s="9">
-        <v>15</v>
+      <c r="E568" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="F568" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G568" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="H568" s="15">
         <v>1</v>
       </c>
       <c r="I568" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G568&amp;", "&amp;H568&amp;"&gt;("&amp;A568&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MAX_VARYING_VECTORS, { { 15 } });</v>
+        <v>requestState&lt;GLboolean, 1&gt;(GL_NORMALIZE, { { GL_FALSE } });</v>
       </c>
       <c r="J568" s="4" t="b">
         <f>TRUE</f>
@@ -26985,20 +26612,20 @@
       </c>
       <c r="L568" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="569" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A569" s="33" t="s">
-        <v>627</v>
+        <v>722</v>
       </c>
       <c r="B569" s="2"/>
       <c r="C569" s="2"/>
       <c r="D569" s="2" t="s">
-        <v>992</v>
+        <v>904</v>
       </c>
       <c r="E569" s="9">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="F569" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
@@ -27012,7 +26639,7 @@
       </c>
       <c r="I569" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G569&amp;", "&amp;H569&amp;"&gt;("&amp;A569&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_MIN_MAP_BUFFER_ALIGNMENT, { { 64 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_NORMAL_ARRAY_BUFFER_BINDING, { { 0 } });</v>
       </c>
       <c r="J569" s="4" t="b">
         <f>TRUE</f>
@@ -27024,34 +26651,34 @@
       </c>
       <c r="L569" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="570" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A570" s="33" t="s">
-        <v>485</v>
+        <v>653</v>
       </c>
       <c r="B570" s="2"/>
       <c r="C570" s="2"/>
       <c r="D570" s="2" t="s">
-        <v>993</v>
-      </c>
-      <c r="E570" s="9" t="s">
-        <v>18</v>
+        <v>994</v>
+      </c>
+      <c r="E570" s="9">
+        <v>4</v>
       </c>
       <c r="F570" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G570" s="1" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="H570" s="15">
         <v>1</v>
       </c>
       <c r="I570" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G570&amp;", "&amp;H570&amp;"&gt;("&amp;A570&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLboolean, 1&gt;(GL_MINMAX, { { GL_FALSE } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_NUM_COMPRESSED_TEXTURE_FORMATS, { { 4 } });</v>
       </c>
       <c r="J570" s="4" t="b">
         <f>TRUE</f>
@@ -27063,36 +26690,30 @@
       </c>
       <c r="L570" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="571" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A571" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B571" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C571" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A571" s="34" t="s">
+        <v>654</v>
+      </c>
+      <c r="B571" s="2"/>
+      <c r="C571" s="2"/>
       <c r="D571" s="2"/>
-      <c r="E571" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="E571" s="9"/>
       <c r="F571" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G571" s="1" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="H571" s="15">
         <v>1</v>
       </c>
       <c r="I571" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G571&amp;", "&amp;H571&amp;"&gt;("&amp;A571&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLboolean, 1&gt;(GL_NORMALIZE, { { GL_FALSE } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_NUM_EXTENSIONS);</v>
       </c>
       <c r="J571" s="4" t="b">
         <f>TRUE</f>
@@ -27104,21 +26725,17 @@
       </c>
       <c r="L571" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="572" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A572" s="33" t="s">
-        <v>722</v>
+      <c r="A572" s="34" t="s">
+        <v>655</v>
       </c>
       <c r="B572" s="2"/>
       <c r="C572" s="2"/>
-      <c r="D572" s="2" t="s">
-        <v>904</v>
-      </c>
-      <c r="E572" s="9">
-        <v>0</v>
-      </c>
+      <c r="D572" s="2"/>
+      <c r="E572" s="9"/>
       <c r="F572" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -27131,7 +26748,7 @@
       </c>
       <c r="I572" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G572&amp;", "&amp;H572&amp;"&gt;("&amp;A572&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_NORMAL_ARRAY_BUFFER_BINDING, { { 0 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_NUM_PROGRAM_BINARY_FORMATS);</v>
       </c>
       <c r="J572" s="4" t="b">
         <f>TRUE</f>
@@ -27143,21 +26760,17 @@
       </c>
       <c r="L572" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="573" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A573" s="33" t="s">
-        <v>653</v>
+      <c r="A573" s="34" t="s">
+        <v>656</v>
       </c>
       <c r="B573" s="2"/>
       <c r="C573" s="2"/>
-      <c r="D573" s="2" t="s">
-        <v>994</v>
-      </c>
-      <c r="E573" s="9">
-        <v>4</v>
-      </c>
+      <c r="D573" s="2"/>
+      <c r="E573" s="9"/>
       <c r="F573" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -27170,7 +26783,7 @@
       </c>
       <c r="I573" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G573&amp;", "&amp;H573&amp;"&gt;("&amp;A573&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_NUM_COMPRESSED_TEXTURE_FORMATS, { { 4 } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_NUM_SHADER_BINARY_FORMATS);</v>
       </c>
       <c r="J573" s="4" t="b">
         <f>TRUE</f>
@@ -27182,30 +26795,34 @@
       </c>
       <c r="L573" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="574" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A574" s="34" t="s">
-        <v>654</v>
+      <c r="A574" s="33" t="s">
+        <v>511</v>
       </c>
       <c r="B574" s="2"/>
       <c r="C574" s="2"/>
-      <c r="D574" s="2"/>
-      <c r="E574" s="9"/>
+      <c r="D574" s="2" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E574" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="F574" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G574" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="H574" s="15">
         <v>1</v>
       </c>
       <c r="I574" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G574&amp;", "&amp;H574&amp;"&gt;("&amp;A574&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_NUM_EXTENSIONS);</v>
+        <v>requestState&lt;GLboolean, 1&gt;(GL_POST_COLOR_MATRIX_COLOR_TABLE, { { GL_FALSE } });</v>
       </c>
       <c r="J574" s="4" t="b">
         <f>TRUE</f>
@@ -27217,30 +26834,34 @@
       </c>
       <c r="L574" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="575" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A575" s="34" t="s">
-        <v>655</v>
+      <c r="A575" s="33" t="s">
+        <v>520</v>
       </c>
       <c r="B575" s="2"/>
       <c r="C575" s="2"/>
-      <c r="D575" s="2"/>
-      <c r="E575" s="9"/>
+      <c r="D575" s="2" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E575" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="F575" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G575" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="H575" s="15">
         <v>1</v>
       </c>
       <c r="I575" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G575&amp;", "&amp;H575&amp;"&gt;("&amp;A575&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_NUM_PROGRAM_BINARY_FORMATS);</v>
+        <v>requestState&lt;GLboolean, 1&gt;(GL_POST_CONVOLUTION_COLOR_TABLE, { { GL_FALSE } });</v>
       </c>
       <c r="J575" s="4" t="b">
         <f>TRUE</f>
@@ -27252,17 +26873,21 @@
       </c>
       <c r="L575" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="576" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A576" s="34" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B576" s="2"/>
       <c r="C576" s="2"/>
-      <c r="D576" s="2"/>
-      <c r="E576" s="9"/>
+      <c r="D576" s="2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E576" s="9">
+        <v>0</v>
+      </c>
       <c r="F576" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -27275,7 +26900,7 @@
       </c>
       <c r="I576" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G576&amp;", "&amp;H576&amp;"&gt;("&amp;A576&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_NUM_SHADER_BINARY_FORMATS);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_PRIMITIVE_RESTART_INDEX, { { 0 } });</v>
       </c>
       <c r="J576" s="4" t="b">
         <f>TRUE</f>
@@ -27287,34 +26912,32 @@
       </c>
       <c r="L576" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="577" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A577" s="33" t="s">
-        <v>511</v>
+      <c r="A577" s="34" t="s">
+        <v>659</v>
       </c>
       <c r="B577" s="2"/>
       <c r="C577" s="2"/>
       <c r="D577" s="2" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E577" s="9" t="s">
-        <v>18</v>
-      </c>
+        <v>1007</v>
+      </c>
+      <c r="E577" s="9"/>
       <c r="F577" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G577" s="1" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="H577" s="15">
         <v>1</v>
       </c>
       <c r="I577" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G577&amp;", "&amp;H577&amp;"&gt;("&amp;A577&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLboolean, 1&gt;(GL_POST_COLOR_MATRIX_COLOR_TABLE, { { GL_FALSE } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_PROGRAM_PIPELINE_BINDING);</v>
       </c>
       <c r="J577" s="4" t="b">
         <f>TRUE</f>
@@ -27326,18 +26949,16 @@
       </c>
       <c r="L577" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="578" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A578" s="33" t="s">
-        <v>520</v>
+      <c r="A578" s="34" t="s">
+        <v>660</v>
       </c>
       <c r="B578" s="2"/>
       <c r="C578" s="2"/>
-      <c r="D578" s="2" t="s">
-        <v>1003</v>
-      </c>
+      <c r="D578" s="2"/>
       <c r="E578" s="9" t="s">
         <v>18</v>
       </c>
@@ -27345,13 +26966,15 @@
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G578" s="1"/>
+      <c r="G578" s="1" t="s">
+        <v>830</v>
+      </c>
       <c r="H578" s="15">
         <v>1</v>
       </c>
       <c r="I578" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G578&amp;", "&amp;H578&amp;"&gt;("&amp;A578&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_POST_CONVOLUTION_COLOR_TABLE, { { GL_FALSE } });</v>
+        <v>requestState&lt;GLboolean, 1&gt;(GL_PROGRAM_POINT_SIZE, { { GL_FALSE } });</v>
       </c>
       <c r="J578" s="4" t="b">
         <f>TRUE</f>
@@ -27363,34 +26986,34 @@
       </c>
       <c r="L578" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="579" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A579" s="34" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="B579" s="2"/>
       <c r="C579" s="2"/>
       <c r="D579" s="2" t="s">
-        <v>1005</v>
-      </c>
-      <c r="E579" s="9">
-        <v>0</v>
+        <v>1006</v>
+      </c>
+      <c r="E579" s="9" t="s">
+        <v>1008</v>
       </c>
       <c r="F579" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G579" s="1" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="H579" s="15">
         <v>1</v>
       </c>
       <c r="I579" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G579&amp;", "&amp;H579&amp;"&gt;("&amp;A579&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_PRIMITIVE_RESTART_INDEX, { { 0 } });</v>
+        <v>requestState&lt;GLenum   , 1&gt;(GL_PROVOKING_VERTEX, { { GL_LAST_VERTEX_CONVENTION } });</v>
       </c>
       <c r="J579" s="4" t="b">
         <f>TRUE</f>
@@ -27402,19 +27025,21 @@
       </c>
       <c r="L579" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="580" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A580" s="34" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="B580" s="2"/>
       <c r="C580" s="2"/>
       <c r="D580" s="2" t="s">
-        <v>1007</v>
-      </c>
-      <c r="E580" s="9"/>
+        <v>1009</v>
+      </c>
+      <c r="E580" s="9">
+        <v>0</v>
+      </c>
       <c r="F580" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -27427,7 +27052,7 @@
       </c>
       <c r="I580" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G580&amp;", "&amp;H580&amp;"&gt;("&amp;A580&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_PROGRAM_PIPELINE_BINDING);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_RENDERBUFFER_BINDING, { { 0 } });</v>
       </c>
       <c r="J580" s="4" t="b">
         <f>TRUE</f>
@@ -27439,19 +27064,17 @@
       </c>
       <c r="L580" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="581" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A581" s="34" t="s">
-        <v>660</v>
+      <c r="A581" s="33" t="s">
+        <v>532</v>
       </c>
       <c r="B581" s="2"/>
       <c r="C581" s="2"/>
       <c r="D581" s="2"/>
-      <c r="E581" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="E581" s="9"/>
       <c r="F581" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -27464,7 +27087,7 @@
       </c>
       <c r="I581" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G581&amp;", "&amp;H581&amp;"&gt;("&amp;A581&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLboolean, 1&gt;(GL_PROGRAM_POINT_SIZE, { { GL_FALSE } });</v>
+        <v>requestState&lt;GLboolean, 1&gt;(GL_RESCALE_NORMAL);</v>
       </c>
       <c r="J581" s="4" t="b">
         <f>TRUE</f>
@@ -27476,34 +27099,34 @@
       </c>
       <c r="L581" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="582" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A582" s="34" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="B582" s="2"/>
       <c r="C582" s="2"/>
       <c r="D582" s="2" t="s">
-        <v>1006</v>
-      </c>
-      <c r="E582" s="9" t="s">
-        <v>1008</v>
+        <v>1010</v>
+      </c>
+      <c r="E582" s="9">
+        <v>0</v>
       </c>
       <c r="F582" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G582" s="1" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="H582" s="15">
         <v>1</v>
       </c>
       <c r="I582" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G582&amp;", "&amp;H582&amp;"&gt;("&amp;A582&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLenum   , 1&gt;(GL_PROVOKING_VERTEX, { { GL_LAST_VERTEX_CONVENTION } });</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_SAMPLER_BINDING, { { 0 } });</v>
       </c>
       <c r="J582" s="4" t="b">
         <f>TRUE</f>
@@ -27515,34 +27138,34 @@
       </c>
       <c r="L582" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="583" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A583" s="34" t="s">
-        <v>662</v>
+      <c r="A583" s="33" t="s">
+        <v>542</v>
       </c>
       <c r="B583" s="2"/>
       <c r="C583" s="2"/>
       <c r="D583" s="2" t="s">
-        <v>1009</v>
-      </c>
-      <c r="E583" s="9">
-        <v>0</v>
+        <v>1015</v>
+      </c>
+      <c r="E583" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="F583" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="G583" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="H583" s="15">
         <v>1</v>
       </c>
       <c r="I583" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G583&amp;", "&amp;H583&amp;"&gt;("&amp;A583&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLint    , 1&gt;(GL_RENDERBUFFER_BINDING, { { 0 } });</v>
+        <v>requestState&lt;GLboolean, 1&gt;(GL_SEPARABLE_2D, { { GL_FALSE } });</v>
       </c>
       <c r="J583" s="4" t="b">
         <f>TRUE</f>
@@ -27554,17 +27177,19 @@
       </c>
       <c r="L583" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="584" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A584" s="33" t="s">
-        <v>532</v>
+      <c r="A584" s="34" t="s">
+        <v>664</v>
       </c>
       <c r="B584" s="2"/>
       <c r="C584" s="2"/>
       <c r="D584" s="2"/>
-      <c r="E584" s="9"/>
+      <c r="E584" s="9" t="s">
+        <v>243</v>
+      </c>
       <c r="F584" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
@@ -27577,7 +27202,7 @@
       </c>
       <c r="I584" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G584&amp;", "&amp;H584&amp;"&gt;("&amp;A584&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLboolean, 1&gt;(GL_RESCALE_NORMAL);</v>
+        <v>requestState&lt;GLboolean, 1&gt;(GL_SHADER_COMPILER, { { GL_TRUE } });</v>
       </c>
       <c r="J584" s="4" t="b">
         <f>TRUE</f>
@@ -27589,30 +27214,30 @@
       </c>
       <c r="L584" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="585" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A585" s="34" t="s">
-        <v>663</v>
+        <v>679</v>
       </c>
       <c r="B585" s="2"/>
       <c r="C585" s="2"/>
-      <c r="D585" s="2" t="s">
-        <v>1010</v>
-      </c>
+      <c r="D585" s="2"/>
       <c r="E585" s="9"/>
       <c r="F585" s="4" t="b">
         <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
         <v>1</v>
       </c>
-      <c r="G585" s="1"/>
+      <c r="G585" s="1" t="s">
+        <v>831</v>
+      </c>
       <c r="H585" s="15">
         <v>1</v>
       </c>
       <c r="I585" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G585&amp;", "&amp;H585&amp;"&gt;("&amp;A585&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, 1&gt;(GL_SAMPLER_BINDING);</v>
+        <v>requestState&lt;GLint    , 1&gt;(GL_TIMESTAMP);</v>
       </c>
       <c r="J585" s="4" t="b">
         <f>TRUE</f>
@@ -27624,83 +27249,81 @@
       </c>
       <c r="L585" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="586" spans="1:12" ht="19.149999999999999" customHeight="1">
+      <c r="A586" s="33" t="s">
+        <v>571</v>
+      </c>
+      <c r="B586" s="10"/>
+      <c r="C586" s="10"/>
+      <c r="D586" s="10"/>
+      <c r="E586" s="28" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="586" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A586" s="33" t="s">
-        <v>542</v>
-      </c>
-      <c r="B586" s="2"/>
-      <c r="C586" s="2"/>
-      <c r="D586" s="2" t="s">
-        <v>1015</v>
-      </c>
-      <c r="E586" s="9" t="s">
+      <c r="F586" s="29" t="b">
+        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
+        <v>1</v>
+      </c>
+      <c r="G586" s="30" t="s">
+        <v>830</v>
+      </c>
+      <c r="H586" s="31">
+        <v>1</v>
+      </c>
+      <c r="I586" s="30" t="str">
+        <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G586&amp;", "&amp;H586&amp;"&gt;("&amp;A586&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
+        <v>requestState&lt;GLboolean, 1&gt;(GL_VERTEX_PROGRAM_POINT_SIZE, { { GL_FALSE } });</v>
+      </c>
+      <c r="J586" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K586" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="L586" s="10">
+        <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="587" spans="1:12" ht="19.149999999999999" customHeight="1">
+      <c r="A587" s="33" t="s">
+        <v>572</v>
+      </c>
+      <c r="B587" s="10"/>
+      <c r="C587" s="10"/>
+      <c r="D587" s="10"/>
+      <c r="E587" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="F586" s="4" t="b">
-        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
-        <v>1</v>
-      </c>
-      <c r="G586" s="1" t="s">
+      <c r="F587" s="29" t="b">
+        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
+        <v>1</v>
+      </c>
+      <c r="G587" s="30" t="s">
         <v>830</v>
       </c>
-      <c r="H586" s="15">
-        <v>1</v>
-      </c>
-      <c r="I586" s="1" t="str">
-        <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G586&amp;", "&amp;H586&amp;"&gt;("&amp;A586&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLboolean, 1&gt;(GL_SEPARABLE_2D, { { GL_FALSE } });</v>
-      </c>
-      <c r="J586" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="K586" s="8" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="L586" s="10">
-        <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="587" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
-      <c r="A587" s="34" t="s">
-        <v>664</v>
-      </c>
-      <c r="B587" s="2"/>
-      <c r="C587" s="2"/>
-      <c r="D587" s="2"/>
-      <c r="E587" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="F587" s="4" t="b">
-        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
-        <v>1</v>
-      </c>
-      <c r="G587" s="1" t="s">
-        <v>830</v>
-      </c>
-      <c r="H587" s="15">
-        <v>1</v>
-      </c>
-      <c r="I587" s="1" t="str">
+      <c r="H587" s="31">
+        <v>1</v>
+      </c>
+      <c r="I587" s="30" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G587&amp;", "&amp;H587&amp;"&gt;("&amp;A587&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;GLboolean, 1&gt;(GL_SHADER_COMPILER, { { GL_TRUE } });</v>
+        <v>requestState&lt;GLboolean, 1&gt;(GL_VERTEX_PROGRAM_TWO_SIDE, { { GL_FALSE } });</v>
       </c>
       <c r="J587" s="4" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="K587" s="8" t="b">
+      <c r="K587" s="32" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="L587" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="588" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
@@ -27771,40 +27394,42 @@
         <v>25</v>
       </c>
     </row>
-    <row r="590" spans="1:12" ht="19.149999999999999" customHeight="1">
-      <c r="A590" s="34" t="s">
-        <v>573</v>
-      </c>
-      <c r="B590" s="10"/>
-      <c r="C590" s="10"/>
-      <c r="D590" s="10"/>
-      <c r="E590" s="28"/>
-      <c r="F590" s="29" t="b">
-        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
-        <v>1</v>
-      </c>
-      <c r="G590" s="30"/>
-      <c r="H590" s="31"/>
-      <c r="I590" s="30" t="str">
+    <row r="590" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
+      <c r="A590" s="33" t="s">
+        <v>599</v>
+      </c>
+      <c r="B590" s="2"/>
+      <c r="C590" s="2"/>
+      <c r="D590" s="2"/>
+      <c r="E590" s="9"/>
+      <c r="F590" s="4" t="b">
+        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
+        <v>1</v>
+      </c>
+      <c r="G590" s="1"/>
+      <c r="H590" s="15">
+        <v>1</v>
+      </c>
+      <c r="I590" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G590&amp;", "&amp;H590&amp;"&gt;("&amp;A590&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
-        <v>requestState&lt;, &gt;(GL_VIEWPORT_INDEX_PROVOKING_VERTEX);</v>
+        <v>requestState&lt;, 1&gt;(GL_MAJOR_VERSION);</v>
       </c>
       <c r="J590" s="4" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="K590" s="32" t="b">
+      <c r="K590" s="8" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="L590" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="591" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
       <c r="A591" s="34" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="B591" s="2"/>
       <c r="C591" s="2"/>
@@ -27820,180 +27445,244 @@
       </c>
       <c r="I591" s="1" t="str">
         <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G591&amp;", "&amp;H591&amp;"&gt;("&amp;A591&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
+        <v>requestState&lt;, 1&gt;(GL_MINOR_VERSION);</v>
+      </c>
+      <c r="J591" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K591" s="8" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="L591" s="10">
+        <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="592" spans="1:12" ht="19.149999999999999" customHeight="1">
+      <c r="A592" s="34" t="s">
+        <v>573</v>
+      </c>
+      <c r="B592" s="10"/>
+      <c r="C592" s="10"/>
+      <c r="D592" s="10"/>
+      <c r="E592" s="28"/>
+      <c r="F592" s="29" t="b">
+        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
+        <v>1</v>
+      </c>
+      <c r="G592" s="30"/>
+      <c r="H592" s="31"/>
+      <c r="I592" s="30" t="str">
+        <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G592&amp;", "&amp;H592&amp;"&gt;("&amp;A592&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
+        <v>requestState&lt;, &gt;(GL_VIEWPORT_INDEX_PROVOKING_VERTEX);</v>
+      </c>
+      <c r="J592" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K592" s="32" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="L592" s="10">
+        <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="593" spans="1:12" ht="19.149999999999999" customHeight="1" outlineLevel="1">
+      <c r="A593" s="34" t="s">
+        <v>658</v>
+      </c>
+      <c r="B593" s="2"/>
+      <c r="C593" s="2"/>
+      <c r="D593" s="2"/>
+      <c r="E593" s="9"/>
+      <c r="F593" s="4" t="b">
+        <f>NOT(ISERROR(VLOOKUP(Table10[enum],Table16[parsed and unfified list of glGet enums from], 1,FALSE)))</f>
+        <v>1</v>
+      </c>
+      <c r="G593" s="1"/>
+      <c r="H593" s="15">
+        <v>1</v>
+      </c>
+      <c r="I593" s="1" t="str">
+        <f>IF(OR(Table10[[#This Row],[status]],NOT(Table10[is enum])),IF(Table10[[#This Row],[is enum]],IF(Table10[[#This Row],[status]],"requestState&lt;"&amp;G593&amp;", "&amp;H593&amp;"&gt;("&amp;A593&amp;IF(ISBLANK(Table10[[#This Row],[default]]),");",(", { { "&amp;Table10[[#This Row],[default]])&amp;" } });")),"std::cout &lt;&lt; std::endl &lt;&lt; """&amp;Table10[[#This Row],[enum]]&amp;""" &lt;&lt; std::endl;"),"")</f>
         <v>requestState&lt;, 1&gt;(GL_PROGRAM_BINARY_FORMATS);</v>
       </c>
-      <c r="J591" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="K591" s="8" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="L591" s="10">
+      <c r="J593" s="4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K593" s="8" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="L593" s="10">
         <f>IF(Table10[[#This Row],[status]],LEN(Table10[[#This Row],[enum]]),"")</f>
         <v>25</v>
       </c>
     </row>
-    <row r="593" spans="1:1" ht="15.75">
-      <c r="A593" s="43"/>
+    <row r="595" spans="1:12" ht="15.75">
+      <c r="A595" s="43"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A272:C273 E272:J273 H304:J307 H311:J312 A311:B312 D311:F312 A304:F307 A330:B331 D330:J331 A542:B542 D542:K542 A292:C293 A296:C296 E296:J296 E292:J293 A294:J295 A297:J303 A274:J291 A313:J329 A332:J348 A349:C354 E349:J354 A308:J310 A355:J458 A459:F460 H459:J460 G459 A461:J462 K272:K462 A2:K271 A463:K479 A480:C481 E480:K481 A588:K591 A587:B587 D587:K587 A543:K586 A482:K541">
-    <cfRule type="expression" dxfId="65" priority="50">
+  <conditionalFormatting sqref="A272:C273 E272:J273 H304:J307 H311:J312 A311:B312 D311:F312 A304:F307 A330:B331 D330:J331 A541:B541 D541:K541 A292:C293 A296:C296 E296:J296 E292:J293 A294:J295 A297:J303 A274:J291 A313:J329 A332:J348 A349:C354 E349:J354 A308:J310 A355:J458 A459:F460 H459:J460 G459 A461:J462 K272:K462 A2:K271 A463:K479 A480:C481 E480:K481 A584:B584 D584:K584 A542:K583 A482:K540 A585:K593">
+    <cfRule type="expression" dxfId="47" priority="50">
       <formula>AND($J2,$K2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="51">
+    <cfRule type="expression" dxfId="46" priority="51">
       <formula>AND($J2,NOT($F2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="52">
+    <cfRule type="expression" dxfId="45" priority="52">
       <formula>NOT($J2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D273 D293 G460">
-    <cfRule type="expression" dxfId="62" priority="155">
+    <cfRule type="expression" dxfId="44" priority="155">
       <formula>AND($J272,$K272)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="156">
+    <cfRule type="expression" dxfId="43" priority="156">
       <formula>AND($J272,NOT($F272))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="157">
+    <cfRule type="expression" dxfId="42" priority="157">
       <formula>NOT($J272)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D272">
-    <cfRule type="expression" dxfId="59" priority="40">
+    <cfRule type="expression" dxfId="41" priority="40">
       <formula>AND($J272,$K272)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="41">
+    <cfRule type="expression" dxfId="40" priority="41">
       <formula>AND($J272,NOT($F272))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="42">
+    <cfRule type="expression" dxfId="39" priority="42">
       <formula>NOT($J272)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G311">
-    <cfRule type="expression" dxfId="56" priority="34">
+    <cfRule type="expression" dxfId="38" priority="34">
       <formula>AND($J312,$K312)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="35">
+    <cfRule type="expression" dxfId="37" priority="35">
       <formula>AND($J312,NOT($F312))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="36">
+    <cfRule type="expression" dxfId="36" priority="36">
       <formula>NOT($J312)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G312">
-    <cfRule type="expression" dxfId="53" priority="31">
+    <cfRule type="expression" dxfId="35" priority="31">
       <formula>AND($J312,$K312)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="32">
+    <cfRule type="expression" dxfId="34" priority="32">
       <formula>AND($J312,NOT($F312))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="33">
+    <cfRule type="expression" dxfId="33" priority="33">
       <formula>NOT($J312)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C311:C312">
-    <cfRule type="expression" dxfId="50" priority="28">
+    <cfRule type="expression" dxfId="32" priority="28">
       <formula>AND($J311,$K311)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="29">
+    <cfRule type="expression" dxfId="31" priority="29">
       <formula>AND($J311,NOT($F311))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="30">
+    <cfRule type="expression" dxfId="30" priority="30">
       <formula>NOT($J311)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G304">
-    <cfRule type="expression" dxfId="47" priority="25">
+    <cfRule type="expression" dxfId="29" priority="25">
       <formula>AND($J304,$K304)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="26">
+    <cfRule type="expression" dxfId="28" priority="26">
       <formula>AND($J304,NOT($F304))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="27">
+    <cfRule type="expression" dxfId="27" priority="27">
       <formula>NOT($J304)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G305">
-    <cfRule type="expression" dxfId="44" priority="22">
+    <cfRule type="expression" dxfId="26" priority="22">
       <formula>AND($J305,$K305)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="23">
+    <cfRule type="expression" dxfId="25" priority="23">
       <formula>AND($J305,NOT($F305))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="24">
+    <cfRule type="expression" dxfId="24" priority="24">
       <formula>NOT($J305)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G306">
-    <cfRule type="expression" dxfId="41" priority="19">
+    <cfRule type="expression" dxfId="23" priority="19">
       <formula>AND($J306,$K306)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="20">
+    <cfRule type="expression" dxfId="22" priority="20">
       <formula>AND($J306,NOT($F306))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="21">
+    <cfRule type="expression" dxfId="21" priority="21">
       <formula>NOT($J306)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G307">
-    <cfRule type="expression" dxfId="38" priority="16">
+    <cfRule type="expression" dxfId="20" priority="16">
       <formula>AND($J307,$K307)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="17">
+    <cfRule type="expression" dxfId="19" priority="17">
       <formula>AND($J307,NOT($F307))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="18">
+    <cfRule type="expression" dxfId="18" priority="18">
       <formula>NOT($J307)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D296">
-    <cfRule type="expression" dxfId="35" priority="10">
+    <cfRule type="expression" dxfId="17" priority="10">
       <formula>AND($J295,$K295)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="11">
+    <cfRule type="expression" dxfId="16" priority="11">
       <formula>AND($J295,NOT($F295))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="12">
+    <cfRule type="expression" dxfId="15" priority="12">
       <formula>NOT($J295)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D292">
-    <cfRule type="expression" dxfId="32" priority="7">
+    <cfRule type="expression" dxfId="14" priority="7">
       <formula>AND($J292,$K292)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="8">
+    <cfRule type="expression" dxfId="13" priority="8">
       <formula>AND($J292,NOT($F292))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="9">
+    <cfRule type="expression" dxfId="12" priority="9">
       <formula>NOT($J292)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C330:C331">
-    <cfRule type="expression" dxfId="29" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>AND($J330,$K330)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>AND($J330,NOT($F330))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="6">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>NOT($J330)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D349:D354">
-    <cfRule type="expression" dxfId="26" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>AND($J349,$K349)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>AND($J349,NOT($F349))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>NOT($J349)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L591">
+  <conditionalFormatting sqref="L2:L593">
     <cfRule type="colorScale" priority="241">
       <colorScale>
         <cfvo type="min"/>
@@ -28004,25 +27693,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D481">
-    <cfRule type="expression" dxfId="23" priority="254">
+    <cfRule type="expression" dxfId="5" priority="254">
       <formula>AND($J495,$K495)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="255">
+    <cfRule type="expression" dxfId="4" priority="255">
       <formula>AND($J495,NOT($F495))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="256">
+    <cfRule type="expression" dxfId="3" priority="256">
       <formula>NOT($J495)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D480">
-    <cfRule type="expression" dxfId="20" priority="275">
-      <formula>AND($J587,$K587)</formula>
+    <cfRule type="expression" dxfId="2" priority="275">
+      <formula>AND($J584,$K584)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="276">
-      <formula>AND($J587,NOT($F587))</formula>
+    <cfRule type="expression" dxfId="1" priority="276">
+      <formula>AND($J584,NOT($F584))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="277">
-      <formula>NOT($J587)</formula>
+    <cfRule type="expression" dxfId="0" priority="277">
+      <formula>NOT($J584)</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>